<commit_message>
Case creator needs a date
</commit_message>
<xml_diff>
--- a/formshare/tests/resources/forms/case/merge/case_start.xlsx
+++ b/formshare/tests/resources/forms/case/merge/case_start.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t xml:space="preserve">canton_id=${canton}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coll_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of collection</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
@@ -386,13 +395,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.69"/>
@@ -478,28 +487,29 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>8</v>
@@ -507,13 +517,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,19 +539,16 @@
       <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>8</v>
@@ -546,7 +556,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>31</v>
@@ -558,10 +568,24 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -579,10 +603,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="5:5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.64"/>
@@ -592,7 +616,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -603,107 +627,107 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -719,36 +743,36 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="5:5 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>